<commit_message>
Added C Clamp to BOM
</commit_message>
<xml_diff>
--- a/Documents/PID_BOM.xlsx
+++ b/Documents/PID_BOM.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t>PID BOM</t>
   </si>
@@ -121,6 +121,12 @@
   </si>
   <si>
     <t>TOTAL</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/Grizzly-H0481-Aluminum-C-Clamps-Opening/dp/B0000DD147/ref=sr_1_31?s=power-hand-tools&amp;ie=UTF8&amp;qid=1476048331&amp;sr=1-31</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Grizzly H0481 Aluminum C-Clamps, Set of 6, 1-Inch Opening </t>
   </si>
 </sst>
 </file>
@@ -542,9 +548,11 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
@@ -749,40 +757,48 @@
       </c>
     </row>
     <row r="16" spans="1:4">
-      <c r="A16" s="2"/>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
+      <c r="A16" s="2">
+        <v>1</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C16" s="2">
+        <v>13.29</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="17" spans="1:4">
-      <c r="A17" s="2">
-        <v>1</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>31</v>
-      </c>
+      <c r="A17" s="2"/>
+      <c r="B17" s="2"/>
       <c r="C17" s="2"/>
-      <c r="D17" s="4" t="s">
-        <v>29</v>
-      </c>
+      <c r="D17" s="2"/>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="2">
         <v>1</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C18" s="2"/>
       <c r="D18" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" s="2">
+        <v>1</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C19" s="2"/>
+      <c r="D19" s="4" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="19" spans="1:4">
-      <c r="A19" s="2"/>
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="2"/>
@@ -792,20 +808,26 @@
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="2"/>
-      <c r="B21" s="3" t="s">
+      <c r="B21" s="2"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" s="2"/>
+      <c r="B22" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C21" s="3">
-        <f>SUM(C4:C15)</f>
-        <v>95.88000000000001</v>
-      </c>
-      <c r="D21" s="2"/>
+      <c r="C22" s="3">
+        <f>SUM(C4:C16)</f>
+        <v>109.17000000000002</v>
+      </c>
+      <c r="D22" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="D17" r:id="rId1"/>
-    <hyperlink ref="D18" r:id="rId2"/>
+    <hyperlink ref="D18" r:id="rId1"/>
+    <hyperlink ref="D19" r:id="rId2"/>
     <hyperlink ref="D15" r:id="rId3"/>
     <hyperlink ref="D14" r:id="rId4"/>
     <hyperlink ref="D4" r:id="rId5"/>

</xml_diff>